<commit_message>
Update on 20210621 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Jobs/20200803开始的新工作作息.xlsx
+++ b/文档/其他文档/Others/Jobs/20200803开始的新工作作息.xlsx
@@ -356,12 +356,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从20210330开始，为了给甘路教训，只需要每两周确认需求。
-即第一周甘路的需求删除了，不需要确认。
-只需求确认第二周的。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>截至2021/5/7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -372,6 +366,13 @@
   </si>
   <si>
     <t>陈勍离职后接手的工作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从20210330开始，为了给甘路教训，只需要每两周确认需求
+即第一周甘路的需求删除了，不需要确认。
+只需求确认第二周的。
+从20210622开始，为了不让施慕垚这个大戆卵话多，除了注明延期理由的需求写在备注里，其余的一概不写。尤其是施慕垚大戆卵的需求！问到就说是来不及开发</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -557,6 +558,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,9 +569,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,13 +923,13 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
       <c r="H3" s="2" t="s">
         <v>75</v>
       </c>
@@ -1127,7 +1128,7 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1317,7 @@
         <v>220</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1337,11 +1338,11 @@
       <c r="E6" s="11">
         <v>247</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>84</v>
+      <c r="F6" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6" s="2">
         <f>I2+I3+I4</f>
@@ -1411,7 +1412,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1429,7 +1430,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1442,16 +1443,16 @@
       <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1471,7 +1472,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>

</xml_diff>